<commit_message>
refactored CreatePlayer with optional parameters, tested with import - working
</commit_message>
<xml_diff>
--- a/Data/Excel/Players-Full-Data - Testing.xlsx
+++ b/Data/Excel/Players-Full-Data - Testing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Grigor</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Sampras</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +743,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>